<commit_message>
updated images and resumes
</commit_message>
<xml_diff>
--- a/_data/research.xlsx
+++ b/_data/research.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu.github.io\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA642F10-0072-4A14-A838-AAEEDD75E58C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADEE03C-F7C4-4ACF-B411-98032014FAF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="24624" windowHeight="15768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Students</t>
   </si>
@@ -43,19 +43,125 @@
   </si>
   <si>
     <t>The objective of this project is to investigate the relationship between deformation of a foldable antenna and effective wavelength. Understanding this association could allow for remote sensing of curvature in flexible robots. Alternatively, the correlation between deformation and effective wavelength could be leveraged to create tunable foldable antennas using closed-loop control techniques.</t>
+  </si>
+  <si>
+    <r>
+      <t>Based on the idea that robots can be made to display many features of animals such as locomotion, the goal of this thesis is to recreate a tail based on the mechanics of a cheetah since the use of its tail is the most effective in dynamic stability and test its effectiveness on an inherently unstable object such as an rc car. The question focuses on which tail design is necessary to fix an inherently unstable object. This topic is derived from how a cheetah uses its tail to stabilize itself while catching prey. The question of developing  a design will be answered by creating a unity model inspired by a cheetah’s tail and simulate how it will stabilize an object that lacks balance. The selected platform is an rc car. The model is already developed in unity, but its movement is not unstable. After making the inherently unstable by adjusting the scaling of the object to make it taller, the motor speed, turning angle, mass of the cube, mass of the wheels, and radius of the wheels, a motor and tail will be added for balance. The selected rc car will be adjusted to match the parameters in unity. The expected result of this procedure is to have a display of a real life model matching the simulation.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Clint Ewell</t>
+  </si>
+  <si>
+    <t>Frank Ononye</t>
+  </si>
+  <si>
+    <t>assets/research/IMG_1261.jpg</t>
+  </si>
+  <si>
+    <t>Sudhanshu Katarey</t>
+  </si>
+  <si>
+    <t>My research draws inspiration from terrestrial avians in terms of development of an optimized leg design for bipedal walking, running and jumping. I will be applying the skills I have learned during the foldable robotics class in the estimation of kinematics, design and fabrication of the robotic leg using software such as Python and SolidWorks. To gauge the dynamics of the leg for different functions I will be using Unity Simulation Engine and Visual Studio to validate the results of experimental testing and biomechanics research.
+My team has already created a model for the leg which we will begin to conduct experiments on. I have used Unity to help test motor parameters in order to select a motor with the best combination of gear ratios, masses and torques for our leg design.</t>
+  </si>
+  <si>
+    <t>Hebellyn Quezada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The purpose of this project is to create a kit that aims to spark an interest in engineering for preadolescents and investigate what are effective methods of doing so. The highlight of this project is the implementation of Choice Theory, which proposes that student engagement increases when they are presented with a series of options to choose from. The kit will consist of lessons that diverge in different directions on multiple steps to represent the diversity of engineering solutions. In the end, these branched out paths will merge together to a single product to show students the interconnectedness of different engineering disciplines. The students’ interaction and completion of the kit will be analyzed to determine what level of complexity and guidance is best suited for preadolescents. 
+</t>
+  </si>
+  <si>
+    <t>assets/research/Hand_prototypes.jpg</t>
+  </si>
+  <si>
+    <t>Children’s Engineering Kit</t>
+  </si>
+  <si>
+    <t>Dante Roush</t>
+  </si>
+  <si>
+    <t>I am expanding the work done by previous Master’s Student Ben Shuch in the field of Quadrupedal Robotic Locomotion. I am utilizing force sensing to calculate the center of balance of a quadrupedal laminate robot with the end goal of implementing a controls system capable of adapting in real time to changing ground angles. Each of the robot’s four legs have two degrees of freedom and are controlled by a four-bar system powered by two servo motors. While standing in place, the robot will behave like a parallel manipulator; when standing on an angled table, it will use the difference between the current force distribution and an ideal force distribution for balance to direct a change in leg length to counteract the angled ground. The laminate materials used to construct the robot make it a more cost effective research platform for researching controls problems.</t>
+  </si>
+  <si>
+    <t>Vipul Gadekar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The projects involve design of wings for a laminate biped robot for providing locomotion stabilization. The wings are designed to provide stabilization for different gait such as running, hopping and jumping. The project aims to develop a reliable dynamics model which includes biped dynamics as well as aerodynamics for creating and testing multiple designs optimized for various gaits. The aerodynamic simulations are run on a vortex-lattice code “VORLAX”, which provides numeric simulation of the defined geometric bodies. The simulations are then to be plugged into the robot dynamics model, which is to be utilized for robot design iterations, simulations and design of a controller. </t>
+  </si>
+  <si>
+    <t>Mohammad Sharifzadeh</t>
+  </si>
+  <si>
+    <t>Yuhao Jiang</t>
+  </si>
+  <si>
+    <t>Shawn (Dongting) Li</t>
+  </si>
+  <si>
+    <t>Roozbeh Khodambashi</t>
+  </si>
+  <si>
+    <t>Mannat Rana</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>archived</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Mobile Soft Robot</t>
+  </si>
+  <si>
+    <t>Octopus-Inspired Hydrogel-based Robots</t>
+  </si>
+  <si>
+    <t>Digging Robot</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Dates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,8 +184,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,34 +468,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="45.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on updating research
</commit_message>
<xml_diff>
--- a/_data/research.xlsx
+++ b/_data/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADEE03C-F7C4-4ACF-B411-98032014FAF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103ADCAD-5CE9-4DBB-9B87-309AAFC7BAFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Students</t>
   </si>
@@ -100,12 +100,6 @@
     <t xml:space="preserve">The projects involve design of wings for a laminate biped robot for providing locomotion stabilization. The wings are designed to provide stabilization for different gait such as running, hopping and jumping. The project aims to develop a reliable dynamics model which includes biped dynamics as well as aerodynamics for creating and testing multiple designs optimized for various gaits. The aerodynamic simulations are run on a vortex-lattice code “VORLAX”, which provides numeric simulation of the defined geometric bodies. The simulations are then to be plugged into the robot dynamics model, which is to be utilized for robot design iterations, simulations and design of a controller. </t>
   </si>
   <si>
-    <t>Mohammad Sharifzadeh</t>
-  </si>
-  <si>
-    <t>Yuhao Jiang</t>
-  </si>
-  <si>
     <t>Shawn (Dongting) Li</t>
   </si>
   <si>
@@ -127,16 +121,106 @@
     <t>Mobile Soft Robot</t>
   </si>
   <si>
-    <t>Octopus-Inspired Hydrogel-based Robots</t>
-  </si>
-  <si>
     <t>Digging Robot</t>
   </si>
   <si>
-    <t>Swimming</t>
-  </si>
-  <si>
     <t>Dates</t>
+  </si>
+  <si>
+    <t>2018-onr/octo1.png</t>
+  </si>
+  <si>
+    <t>We are working to create a framework for design, rapid prototyping and control of robust, energy-efficient, autonomous soft arms with octopus-inspired distributed neuromuscular sensing and actuation. The arms will be capable of continuous deformation through the use of hydrogel "muscles" and distributed sensing through the use of embedded silver "neuron" interconnections. Such a unique octopus-inspired design forms a built-in local "sensing-actuation" feedback loop to achieve adaptive reconfiguration in response to the local environment. Such local adaptation will enable the robot to perform high-level tasks such as locomotion and reversible adhesion without coordination from a central controller in a highly accurate, rapid, and energy-efficient way. This study will also produce fundamental principles and theory for the modeling and control of soft robots in a way which leverages their unique capabilities and is inspired by how cephalopod appendages interact with their environment.</t>
+  </si>
+  <si>
+    <t>Buoyancy Control of a Bio-inspired Robotic Fish</t>
+  </si>
+  <si>
+    <t>Alia Gilbert</t>
+  </si>
+  <si>
+    <t>This project focuses on controlling the altitude of an underwater robot meant to do environmental cleanup of vegetation in a canal. A bladder modeled off fish anatomy will be designed containing two bulbs, likely of laminate material, with a tube containing a pump. The pump will transfer air between the two bulbs to control the direction of the buoyancy in the robot. The shift in buoyancy will allow the body of the robot to move either up or down. Using this laminate material in prototyping for underwater robotics allows for low cost testing and quick turnaround time for iterations. We will be checking consistency of the level that the robot is driving using an IMU to control the amount of water or air in the bulbs of the systems.</t>
+  </si>
+  <si>
+    <t>Design of a Hopping Platform using Laminate Construction</t>
+  </si>
+  <si>
+    <t>Jacob Knaup</t>
+  </si>
+  <si>
+    <t>2017-knaup-jumping/render.png</t>
+  </si>
+  <si>
+    <t>Taking advantage of laminate materials' flexibility, a high-performance jumping platform is developed. A physical prototype and accurate model of the design are sought in tandem with each being used to inform the other. This will result in a leg design to be incorporated into future jumping or hopping robots and a validated simulation that can be used to design future robots using the same methods.</t>
+  </si>
+  <si>
+    <t>Underactuated Laminate gripper with Low-Cost Sensing.</t>
+  </si>
+  <si>
+    <t>Drew Carlson</t>
+  </si>
+  <si>
+    <t>2017-underactuated-hand/picture1.png</t>
+  </si>
+  <si>
+    <t>This project explores the design and development of a robotic gripper using low cost materials. It uses a four-bar mechanism to grasp objects. The system is back driven until the finger makes contact with an object. The servo continues to drive over coming the force of a spring holding the gripper in a open position providing the method of under-actuation.   The laminate design allows for multiple materials to be used. This can be exploited to make the contact points more flexible for the inclusion of flex sensors. By using multiple low cost flex sensors the location, number, and amount of force being applied in the grip can be determined using beam theory as a model.</t>
+  </si>
+  <si>
+    <t>Fish-Inspired Robot for Navigating Tight Spaces</t>
+  </si>
+  <si>
+    <t>Mohammad Sharifzadeh, Yuhao Jiang</t>
+  </si>
+  <si>
+    <t>fixed-fish.png</t>
+  </si>
+  <si>
+    <t>In this project, the goal is to build an AUV that explores the water canals and performs cleaning of these canals as necessary. We have selected the fin propulsion mechanism as the propulsion system for our AUV. Essentially, we are designing and building an underwater robot that will use a fin to move inside water. Our capability of using a laminated robot, will give us more advantage in easily gain the required stiffness in the tail in order to overcome the water drag. This work is supported in part by Salt River Project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Design, Implementation, and Testing of a Force-Sensing Quadrupedal Laminate Robot</t>
+  </si>
+  <si>
+    <t>Ben Shuch</t>
+  </si>
+  <si>
+    <t>shuch-project.jpg</t>
+  </si>
+  <si>
+    <t>In this project we present a low-cost force-sensing quadrupedal laminate robot platform. The robot has two degrees of freedom on each of four independent legs, allowing for a variety of motion trajectories to be created at each leg, thus creating a rich control space to explore on a relatively low-cost robot. This platform will allow a user to research complex motion and gait analysis control questions, and use different concepts in computer science and control theory methods to permit  it to walk.   The motion trajectory of each leg has been modeled in Python. Critical design considerations are the complexity of the laminate design, the rigidity of the materials of which the laminate is constructed, the accuracy of the transmission to control each leg, and the design of the force sensing legs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Development of an Multi-Process Planning Tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fab3-1.png</t>
+  </si>
+  <si>
+    <t>Cole Brauer</t>
+  </si>
+  <si>
+    <t>This project is researching methods of automating the planning of multi-material manufacturing processes.  This research will be used to inform the development of a software planning tool that would aid in the development of low-cost educational robots.  The focus of this project is on processes that are widely available in educational institutions such as 3D printing and laser cutting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Low-Cost, Modular Force Control Solution</t>
+  </si>
+  <si>
+    <t>2017-knaup-force-sensing/springy-four-bar.png</t>
+  </si>
+  <si>
+    <t>Force control offers numerous benefits to robots over other control schemes such as more natural movements and increased sensitivity to the surrounding environment, but it is typically only available to high-end robots. This research aims to develop a modular force control solution for low-cost robots. The solution is designed to be easy to incorporate into future laminate robots, allowing the designer to add force control capabilities, while placing minimal constraints on the design.</t>
+  </si>
+  <si>
+    <t>Design of a Cutting Tool for Clearing Underwater Vegetation</t>
+  </si>
+  <si>
+    <t>Sheena Benson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The objective of this research is to further the development of the bio-inspired fish being and constructed by Dr. Aukes and his team of student researchers by designing an inexpensive, reliable, and effective cutting tool to be used in conjunction with the robotic fish to cut and reduce the number of underwater vegetation growing in canals and waterways here in Phoenix. Such a device would reduce the cost and manpower currently used to clear those canals. Without clearing aquatic plants from the canals, certain parts of the city would also become vulnerable to increased flooding in the event of a sudden downpour, leading to possible infrastructure damage. </t>
+  </si>
+  <si>
+    <t>Octopus-Inspired Soft Hydrogel Robots</t>
   </si>
 </sst>
 </file>
@@ -468,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,10 +582,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -562,95 +646,163 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="1" t="s">
-        <v>27</v>
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>